<commit_message>
added dummy reiviews files and charts generation with sentiment analysis
</commit_message>
<xml_diff>
--- a/review_sentiments.xlsx
+++ b/review_sentiments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,19 +448,19 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>101	Wireless Mouse	Alice	5	Great mouse, very responsive!</t>
+          <t>i dont liek teh product,</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>POSITIVE</t>
+          <t>NEGATIVE</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>101	Wireless Mouse	Bob	4	Good value for money</t>
+          <t>i love it , its wonderful , it exceeded my expectations</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,7 +472,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>102	Bluetooth Headphones	Charlie	3	Sound quality is decent but could be better</t>
+          <t>Battery life could be better.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>102	Bluetooth Headphones	Diana	5	Excellent headphones, love the bass!</t>
+          <t>Excellent quality, highly recommend!</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>103	Mechanical Keyboard	Ethan	4	Solid build and satisfying typing experience</t>
+          <t>Durable and worth the money.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>103	Mechanical Keyboard	Fiona	5	Best keyboard I've ever used</t>
+          <t>Excellent quality, highly recommend!</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,7 +520,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>104	4K Monitor	George	4	Crisp display with vibrant colors</t>
+          <t>Would definitely buy again.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>105	Smartphone Case	Hannah	3	Case is okay, but feels a bit cheap</t>
+          <t>Battery life could be better.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>Would definitely buy again.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,19 +556,19 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>Not as expected, a bit disappointed.</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>POSITIVE</t>
+          <t>NEGATIVE</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>Amazing performance and design.</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>Fast delivery and good packaging.</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,19 +592,19 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>Battery life could be better.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>POSITIVE</t>
+          <t>NEGATIVE</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>Good value for the price.</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -616,7 +616,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>Exceeded my expectations!</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,7 +628,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>107</t>
+          <t>Very comfortable to use.</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -640,7 +640,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>Durable and worth the money.</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>Very comfortable to use.</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>Amazing performance and design.</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>107</t>
+          <t>Very comfortable to use.</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -688,7 +688,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>Would definitely buy again.</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -700,19 +700,19 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>Not as expected, a bit disappointed.</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>POSITIVE</t>
+          <t>NEGATIVE</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>Durable and worth the money.</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>Good value for the price.</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -736,7 +736,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>Fast delivery and good packaging.</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -748,19 +748,19 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>Battery life could be better.</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>POSITIVE</t>
+          <t>NEGATIVE</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>Fast delivery and good packaging.</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -772,7 +772,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>Amazing performance and design.</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>Durable and worth the money.</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -796,7 +796,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>Durable and worth the money.</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>Excellent quality, highly recommend!</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -820,7 +820,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>Very comfortable to use.</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -832,7 +832,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>102</t>
+          <t>Excellent quality, highly recommend!</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -844,7 +844,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>Very comfortable to use.</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -856,7 +856,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>Excellent quality, highly recommend!</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -868,19 +868,19 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>Battery life could be better.</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>POSITIVE</t>
+          <t>NEGATIVE</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>Amazing performance and design.</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -892,7 +892,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>Exceeded my expectations!</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -904,7 +904,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>Would definitely buy again.</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -916,7 +916,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>Durable and worth the money.</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -928,7 +928,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>Fast delivery and good packaging.</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -940,7 +940,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>105</t>
+          <t>Excellent quality, highly recommend!</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -952,7 +952,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>Good value for the price.</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>Very comfortable to use.</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -976,7 +976,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>103</t>
+          <t>Excellent quality, highly recommend!</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -988,19 +988,19 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>108</t>
+          <t>Not as expected, a bit disappointed.</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>POSITIVE</t>
+          <t>NEGATIVE</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>Durable and worth the money.</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1012,7 +1012,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>Exceeded my expectations!</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1024,7 +1024,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>106</t>
+          <t>Would definitely buy again.</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1036,7 +1036,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>104</t>
+          <t>Very comfortable to use.</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1048,7 +1048,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>101</t>
+          <t>Very comfortable to use.</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1060,82 +1060,10 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>109</t>
+          <t>Durable and worth the money.</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
-        <is>
-          <t>POSITIVE</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>110</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>POSITIVE</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>106</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>POSITIVE</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>108</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>POSITIVE</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>101</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>POSITIVE</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>109</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>POSITIVE</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>104</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
         <is>
           <t>POSITIVE</t>
         </is>

</xml_diff>